<commit_message>
added all available MGTs except C2C
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/link_map_vu13p_gty.xlsx
+++ b/examples/vu13p_25g_all/src/link_map_vu13p_gty.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="30">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X0Y24 AXI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X0Y30 AXI</t>
   </si>
 </sst>
 </file>
@@ -234,10 +240,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H244"/>
+  <dimension ref="A1:I256"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A224" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7:H244"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -245,10 +251,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.29"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.87"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="9" style="2" width="11.52"/>
   </cols>
   <sheetData>
@@ -1629,6 +1635,9 @@
         <f aca="false">H50+1</f>
         <v>23</v>
       </c>
+      <c r="I52" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
@@ -1638,7 +1647,7 @@
         <v>0</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>15</v>
@@ -1665,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>15</v>
@@ -1692,7 +1701,7 @@
         <v>0</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>15</v>
@@ -1719,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>15</v>
@@ -1746,7 +1755,7 @@
         <v>0</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>15</v>
@@ -1773,7 +1782,7 @@
         <v>0</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>15</v>
@@ -1800,7 +1809,7 @@
         <v>0</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>15</v>
@@ -1827,7 +1836,7 @@
         <v>0</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>15</v>
@@ -1854,7 +1863,7 @@
         <v>0</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>15</v>
@@ -1881,7 +1890,7 @@
         <v>0</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>15</v>
@@ -1899,6 +1908,9 @@
         <f aca="false">H60+1</f>
         <v>28</v>
       </c>
+      <c r="I62" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
@@ -1908,7 +1920,7 @@
         <v>0</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>15</v>
@@ -1935,7 +1947,7 @@
         <v>0</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>15</v>
@@ -1953,6 +1965,7 @@
         <f aca="false">H62+1</f>
         <v>29</v>
       </c>
+      <c r="I64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
@@ -1962,7 +1975,7 @@
         <v>0</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>15</v>
@@ -1989,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>15</v>
@@ -2016,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>15</v>
@@ -2043,7 +2056,7 @@
         <v>0</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>15</v>
@@ -2070,7 +2083,7 @@
         <v>0</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>15</v>
@@ -2097,7 +2110,7 @@
         <v>0</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>15</v>
@@ -2124,7 +2137,7 @@
         <v>0</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>15</v>
@@ -2151,7 +2164,7 @@
         <v>0</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>15</v>
@@ -2178,7 +2191,7 @@
         <v>0</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>15</v>
@@ -2205,7 +2218,7 @@
         <v>0</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>15</v>
@@ -2232,7 +2245,7 @@
         <v>0</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>15</v>
@@ -2259,7 +2272,7 @@
         <v>0</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>15</v>
@@ -2286,7 +2299,7 @@
         <v>0</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>15</v>
@@ -2313,7 +2326,7 @@
         <v>0</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>15</v>
@@ -2340,7 +2353,7 @@
         <v>0</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>15</v>
@@ -2367,7 +2380,7 @@
         <v>0</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>15</v>
@@ -2394,7 +2407,7 @@
         <v>0</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>15</v>
@@ -2421,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>15</v>
@@ -2448,7 +2461,7 @@
         <v>0</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>15</v>
@@ -2475,7 +2488,7 @@
         <v>0</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>15</v>
@@ -2502,7 +2515,7 @@
         <v>0</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>15</v>
@@ -2529,7 +2542,7 @@
         <v>0</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>15</v>
@@ -2556,7 +2569,7 @@
         <v>0</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>15</v>
@@ -2583,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>15</v>
@@ -2610,7 +2623,7 @@
         <v>0</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>15</v>
@@ -2637,7 +2650,7 @@
         <v>0</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>15</v>
@@ -2664,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>15</v>
@@ -2691,7 +2704,7 @@
         <v>0</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>15</v>
@@ -2718,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>15</v>
@@ -2745,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>15</v>
@@ -2772,7 +2785,7 @@
         <v>0</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>15</v>
@@ -2799,7 +2812,7 @@
         <v>0</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>15</v>
@@ -2826,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>15</v>
@@ -2853,7 +2866,7 @@
         <v>0</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>15</v>
@@ -2880,7 +2893,7 @@
         <v>0</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>15</v>
@@ -2907,7 +2920,7 @@
         <v>0</v>
       </c>
       <c r="C100" s="1" t="n">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>15</v>
@@ -2934,7 +2947,7 @@
         <v>0</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>15</v>
@@ -2961,7 +2974,7 @@
         <v>0</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>15</v>
@@ -2988,7 +3001,7 @@
         <v>0</v>
       </c>
       <c r="C103" s="1" t="n">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>15</v>
@@ -3015,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="C104" s="1" t="n">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>15</v>
@@ -3042,7 +3055,7 @@
         <v>0</v>
       </c>
       <c r="C105" s="1" t="n">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>15</v>
@@ -3069,7 +3082,7 @@
         <v>0</v>
       </c>
       <c r="C106" s="1" t="n">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>15</v>
@@ -3096,7 +3109,7 @@
         <v>0</v>
       </c>
       <c r="C107" s="1" t="n">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>15</v>
@@ -3123,7 +3136,7 @@
         <v>0</v>
       </c>
       <c r="C108" s="1" t="n">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>15</v>
@@ -3150,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="C109" s="1" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>15</v>
@@ -3177,7 +3190,7 @@
         <v>0</v>
       </c>
       <c r="C110" s="1" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>15</v>
@@ -3204,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="C111" s="1" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>15</v>
@@ -3231,7 +3244,7 @@
         <v>0</v>
       </c>
       <c r="C112" s="1" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>15</v>
@@ -3258,7 +3271,7 @@
         <v>0</v>
       </c>
       <c r="C113" s="1" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>15</v>
@@ -3285,7 +3298,7 @@
         <v>0</v>
       </c>
       <c r="C114" s="1" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>15</v>
@@ -3312,7 +3325,7 @@
         <v>0</v>
       </c>
       <c r="C115" s="1" t="n">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>15</v>
@@ -3339,7 +3352,7 @@
         <v>0</v>
       </c>
       <c r="C116" s="1" t="n">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>15</v>
@@ -3363,10 +3376,10 @@
         <v>13</v>
       </c>
       <c r="B117" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C117" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
+      </c>
+      <c r="C117" s="1" t="n">
+        <v>58</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>15</v>
@@ -3390,10 +3403,10 @@
         <v>19</v>
       </c>
       <c r="B118" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C118" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
+      </c>
+      <c r="C118" s="1" t="n">
+        <v>58</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>15</v>
@@ -3417,10 +3430,10 @@
         <v>13</v>
       </c>
       <c r="B119" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
+      </c>
+      <c r="C119" s="1" t="n">
+        <v>59</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>15</v>
@@ -3444,10 +3457,10 @@
         <v>19</v>
       </c>
       <c r="B120" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>21</v>
+        <v>0</v>
+      </c>
+      <c r="C120" s="1" t="n">
+        <v>59</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>15</v>
@@ -3471,10 +3484,10 @@
         <v>13</v>
       </c>
       <c r="B121" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="C121" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>15</v>
@@ -3498,10 +3511,10 @@
         <v>19</v>
       </c>
       <c r="B122" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C122" s="1" t="s">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="C122" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>15</v>
@@ -3525,10 +3538,10 @@
         <v>13</v>
       </c>
       <c r="B123" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="C123" s="1" t="n">
+        <v>61</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>15</v>
@@ -3552,10 +3565,10 @@
         <v>19</v>
       </c>
       <c r="B124" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C124" s="1" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+      <c r="C124" s="1" t="n">
+        <v>61</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>15</v>
@@ -3579,10 +3592,10 @@
         <v>13</v>
       </c>
       <c r="B125" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C125" s="1" t="s">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="C125" s="1" t="n">
+        <v>62</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>15</v>
@@ -3606,10 +3619,10 @@
         <v>19</v>
       </c>
       <c r="B126" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>24</v>
+        <v>0</v>
+      </c>
+      <c r="C126" s="1" t="n">
+        <v>62</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>15</v>
@@ -3633,10 +3646,10 @@
         <v>13</v>
       </c>
       <c r="B127" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="C127" s="1" t="n">
+        <v>63</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>15</v>
@@ -3660,10 +3673,10 @@
         <v>19</v>
       </c>
       <c r="B128" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>25</v>
+        <v>0</v>
+      </c>
+      <c r="C128" s="1" t="n">
+        <v>63</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>15</v>
@@ -3690,7 +3703,7 @@
         <v>1</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>15</v>
@@ -3717,7 +3730,7 @@
         <v>1</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>15</v>
@@ -3744,7 +3757,7 @@
         <v>1</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>15</v>
@@ -3771,7 +3784,7 @@
         <v>1</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>15</v>
@@ -3797,8 +3810,8 @@
       <c r="B133" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C133" s="1" t="n">
-        <v>8</v>
+      <c r="C133" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>15</v>
@@ -3824,8 +3837,8 @@
       <c r="B134" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C134" s="1" t="n">
-        <v>8</v>
+      <c r="C134" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="D134" s="1" t="s">
         <v>15</v>
@@ -3851,8 +3864,8 @@
       <c r="B135" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C135" s="1" t="n">
-        <v>9</v>
+      <c r="C135" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D135" s="1" t="s">
         <v>15</v>
@@ -3878,8 +3891,8 @@
       <c r="B136" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C136" s="1" t="n">
-        <v>9</v>
+      <c r="C136" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="D136" s="1" t="s">
         <v>15</v>
@@ -3905,8 +3918,8 @@
       <c r="B137" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C137" s="1" t="n">
-        <v>10</v>
+      <c r="C137" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D137" s="1" t="s">
         <v>15</v>
@@ -3932,8 +3945,8 @@
       <c r="B138" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C138" s="1" t="n">
-        <v>10</v>
+      <c r="C138" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="D138" s="1" t="s">
         <v>15</v>
@@ -3959,8 +3972,8 @@
       <c r="B139" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C139" s="1" t="n">
-        <v>11</v>
+      <c r="C139" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D139" s="1" t="s">
         <v>15</v>
@@ -3986,8 +3999,8 @@
       <c r="B140" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C140" s="1" t="n">
-        <v>11</v>
+      <c r="C140" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="D140" s="1" t="s">
         <v>15</v>
@@ -4013,8 +4026,8 @@
       <c r="B141" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C141" s="1" t="n">
-        <v>12</v>
+      <c r="C141" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D141" s="1" t="s">
         <v>15</v>
@@ -4040,8 +4053,8 @@
       <c r="B142" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C142" s="1" t="n">
-        <v>12</v>
+      <c r="C142" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="D142" s="1" t="s">
         <v>15</v>
@@ -4067,8 +4080,8 @@
       <c r="B143" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C143" s="1" t="n">
-        <v>13</v>
+      <c r="C143" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D143" s="1" t="s">
         <v>15</v>
@@ -4094,8 +4107,8 @@
       <c r="B144" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C144" s="1" t="n">
-        <v>13</v>
+      <c r="C144" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D144" s="1" t="s">
         <v>15</v>
@@ -4122,7 +4135,7 @@
         <v>1</v>
       </c>
       <c r="C145" s="1" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D145" s="1" t="s">
         <v>15</v>
@@ -4149,7 +4162,7 @@
         <v>1</v>
       </c>
       <c r="C146" s="1" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D146" s="1" t="s">
         <v>15</v>
@@ -4176,7 +4189,7 @@
         <v>1</v>
       </c>
       <c r="C147" s="1" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>15</v>
@@ -4203,7 +4216,7 @@
         <v>1</v>
       </c>
       <c r="C148" s="1" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D148" s="1" t="s">
         <v>15</v>
@@ -4230,7 +4243,7 @@
         <v>1</v>
       </c>
       <c r="C149" s="1" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D149" s="1" t="s">
         <v>15</v>
@@ -4257,7 +4270,7 @@
         <v>1</v>
       </c>
       <c r="C150" s="1" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D150" s="1" t="s">
         <v>15</v>
@@ -4284,7 +4297,7 @@
         <v>1</v>
       </c>
       <c r="C151" s="1" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D151" s="1" t="s">
         <v>15</v>
@@ -4311,7 +4324,7 @@
         <v>1</v>
       </c>
       <c r="C152" s="1" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D152" s="1" t="s">
         <v>15</v>
@@ -4338,7 +4351,7 @@
         <v>1</v>
       </c>
       <c r="C153" s="1" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D153" s="1" t="s">
         <v>15</v>
@@ -4365,7 +4378,7 @@
         <v>1</v>
       </c>
       <c r="C154" s="1" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D154" s="1" t="s">
         <v>15</v>
@@ -4392,7 +4405,7 @@
         <v>1</v>
       </c>
       <c r="C155" s="1" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D155" s="1" t="s">
         <v>15</v>
@@ -4419,7 +4432,7 @@
         <v>1</v>
       </c>
       <c r="C156" s="1" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D156" s="1" t="s">
         <v>15</v>
@@ -4446,7 +4459,7 @@
         <v>1</v>
       </c>
       <c r="C157" s="1" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D157" s="1" t="s">
         <v>15</v>
@@ -4473,7 +4486,7 @@
         <v>1</v>
       </c>
       <c r="C158" s="1" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="D158" s="1" t="s">
         <v>15</v>
@@ -4500,7 +4513,7 @@
         <v>1</v>
       </c>
       <c r="C159" s="1" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D159" s="1" t="s">
         <v>15</v>
@@ -4527,7 +4540,7 @@
         <v>1</v>
       </c>
       <c r="C160" s="1" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D160" s="1" t="s">
         <v>15</v>
@@ -4554,7 +4567,7 @@
         <v>1</v>
       </c>
       <c r="C161" s="1" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D161" s="1" t="s">
         <v>15</v>
@@ -4581,7 +4594,7 @@
         <v>1</v>
       </c>
       <c r="C162" s="1" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D162" s="1" t="s">
         <v>15</v>
@@ -4608,7 +4621,7 @@
         <v>1</v>
       </c>
       <c r="C163" s="1" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D163" s="1" t="s">
         <v>15</v>
@@ -4635,7 +4648,7 @@
         <v>1</v>
       </c>
       <c r="C164" s="1" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D164" s="1" t="s">
         <v>15</v>
@@ -4662,7 +4675,7 @@
         <v>1</v>
       </c>
       <c r="C165" s="1" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>15</v>
@@ -4689,7 +4702,7 @@
         <v>1</v>
       </c>
       <c r="C166" s="1" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>15</v>
@@ -4716,7 +4729,7 @@
         <v>1</v>
       </c>
       <c r="C167" s="1" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D167" s="1" t="s">
         <v>15</v>
@@ -4743,7 +4756,7 @@
         <v>1</v>
       </c>
       <c r="C168" s="1" t="n">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D168" s="1" t="s">
         <v>15</v>
@@ -4770,7 +4783,7 @@
         <v>1</v>
       </c>
       <c r="C169" s="1" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D169" s="1" t="s">
         <v>15</v>
@@ -4797,7 +4810,7 @@
         <v>1</v>
       </c>
       <c r="C170" s="1" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D170" s="1" t="s">
         <v>15</v>
@@ -4824,7 +4837,7 @@
         <v>1</v>
       </c>
       <c r="C171" s="1" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>15</v>
@@ -4851,7 +4864,7 @@
         <v>1</v>
       </c>
       <c r="C172" s="1" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>15</v>
@@ -4878,7 +4891,7 @@
         <v>1</v>
       </c>
       <c r="C173" s="1" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D173" s="1" t="s">
         <v>15</v>
@@ -4905,7 +4918,7 @@
         <v>1</v>
       </c>
       <c r="C174" s="1" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D174" s="1" t="s">
         <v>15</v>
@@ -4932,7 +4945,7 @@
         <v>1</v>
       </c>
       <c r="C175" s="1" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D175" s="1" t="s">
         <v>15</v>
@@ -4959,7 +4972,7 @@
         <v>1</v>
       </c>
       <c r="C176" s="1" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D176" s="1" t="s">
         <v>15</v>
@@ -4986,7 +4999,7 @@
         <v>1</v>
       </c>
       <c r="C177" s="1" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D177" s="1" t="s">
         <v>15</v>
@@ -5013,7 +5026,7 @@
         <v>1</v>
       </c>
       <c r="C178" s="1" t="n">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>15</v>
@@ -5040,7 +5053,7 @@
         <v>1</v>
       </c>
       <c r="C179" s="1" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>15</v>
@@ -5067,7 +5080,7 @@
         <v>1</v>
       </c>
       <c r="C180" s="1" t="n">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D180" s="1" t="s">
         <v>15</v>
@@ -5094,7 +5107,7 @@
         <v>1</v>
       </c>
       <c r="C181" s="1" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>15</v>
@@ -5121,7 +5134,7 @@
         <v>1</v>
       </c>
       <c r="C182" s="1" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>15</v>
@@ -5148,7 +5161,7 @@
         <v>1</v>
       </c>
       <c r="C183" s="1" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>15</v>
@@ -5175,7 +5188,7 @@
         <v>1</v>
       </c>
       <c r="C184" s="1" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>15</v>
@@ -5202,7 +5215,7 @@
         <v>1</v>
       </c>
       <c r="C185" s="1" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>15</v>
@@ -5229,7 +5242,7 @@
         <v>1</v>
       </c>
       <c r="C186" s="1" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>15</v>
@@ -5256,7 +5269,7 @@
         <v>1</v>
       </c>
       <c r="C187" s="1" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D187" s="1" t="s">
         <v>15</v>
@@ -5283,7 +5296,7 @@
         <v>1</v>
       </c>
       <c r="C188" s="1" t="n">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>15</v>
@@ -5310,7 +5323,7 @@
         <v>1</v>
       </c>
       <c r="C189" s="1" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D189" s="1" t="s">
         <v>15</v>
@@ -5337,7 +5350,7 @@
         <v>1</v>
       </c>
       <c r="C190" s="1" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>15</v>
@@ -5364,7 +5377,7 @@
         <v>1</v>
       </c>
       <c r="C191" s="1" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>15</v>
@@ -5391,7 +5404,7 @@
         <v>1</v>
       </c>
       <c r="C192" s="1" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>15</v>
@@ -5418,7 +5431,7 @@
         <v>1</v>
       </c>
       <c r="C193" s="1" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>15</v>
@@ -5445,7 +5458,7 @@
         <v>1</v>
       </c>
       <c r="C194" s="1" t="n">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>15</v>
@@ -5472,7 +5485,7 @@
         <v>1</v>
       </c>
       <c r="C195" s="1" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>15</v>
@@ -5499,7 +5512,7 @@
         <v>1</v>
       </c>
       <c r="C196" s="1" t="n">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D196" s="1" t="s">
         <v>15</v>
@@ -5526,7 +5539,7 @@
         <v>1</v>
       </c>
       <c r="C197" s="1" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D197" s="1" t="s">
         <v>15</v>
@@ -5553,7 +5566,7 @@
         <v>1</v>
       </c>
       <c r="C198" s="1" t="n">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D198" s="1" t="s">
         <v>15</v>
@@ -5580,7 +5593,7 @@
         <v>1</v>
       </c>
       <c r="C199" s="1" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D199" s="1" t="s">
         <v>15</v>
@@ -5607,7 +5620,7 @@
         <v>1</v>
       </c>
       <c r="C200" s="1" t="n">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D200" s="1" t="s">
         <v>15</v>
@@ -5634,7 +5647,7 @@
         <v>1</v>
       </c>
       <c r="C201" s="1" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D201" s="1" t="s">
         <v>15</v>
@@ -5661,7 +5674,7 @@
         <v>1</v>
       </c>
       <c r="C202" s="1" t="n">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>15</v>
@@ -5688,7 +5701,7 @@
         <v>1</v>
       </c>
       <c r="C203" s="1" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D203" s="1" t="s">
         <v>15</v>
@@ -5715,7 +5728,7 @@
         <v>1</v>
       </c>
       <c r="C204" s="1" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>15</v>
@@ -5742,7 +5755,7 @@
         <v>1</v>
       </c>
       <c r="C205" s="1" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>15</v>
@@ -5769,7 +5782,7 @@
         <v>1</v>
       </c>
       <c r="C206" s="1" t="n">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>15</v>
@@ -5796,7 +5809,7 @@
         <v>1</v>
       </c>
       <c r="C207" s="1" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>15</v>
@@ -5823,7 +5836,7 @@
         <v>1</v>
       </c>
       <c r="C208" s="1" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D208" s="1" t="s">
         <v>15</v>
@@ -5850,7 +5863,7 @@
         <v>1</v>
       </c>
       <c r="C209" s="1" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D209" s="1" t="s">
         <v>15</v>
@@ -5877,7 +5890,7 @@
         <v>1</v>
       </c>
       <c r="C210" s="1" t="n">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D210" s="1" t="s">
         <v>15</v>
@@ -5904,7 +5917,7 @@
         <v>1</v>
       </c>
       <c r="C211" s="1" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D211" s="1" t="s">
         <v>15</v>
@@ -5931,7 +5944,7 @@
         <v>1</v>
       </c>
       <c r="C212" s="1" t="n">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D212" s="1" t="s">
         <v>15</v>
@@ -5958,7 +5971,7 @@
         <v>1</v>
       </c>
       <c r="C213" s="1" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D213" s="1" t="s">
         <v>15</v>
@@ -5985,7 +5998,7 @@
         <v>1</v>
       </c>
       <c r="C214" s="1" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D214" s="1" t="s">
         <v>15</v>
@@ -6012,7 +6025,7 @@
         <v>1</v>
       </c>
       <c r="C215" s="1" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D215" s="1" t="s">
         <v>15</v>
@@ -6039,7 +6052,7 @@
         <v>1</v>
       </c>
       <c r="C216" s="1" t="n">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D216" s="1" t="s">
         <v>15</v>
@@ -6066,7 +6079,7 @@
         <v>1</v>
       </c>
       <c r="C217" s="1" t="n">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D217" s="1" t="s">
         <v>15</v>
@@ -6093,7 +6106,7 @@
         <v>1</v>
       </c>
       <c r="C218" s="1" t="n">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="D218" s="1" t="s">
         <v>15</v>
@@ -6120,7 +6133,7 @@
         <v>1</v>
       </c>
       <c r="C219" s="1" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D219" s="1" t="s">
         <v>15</v>
@@ -6147,7 +6160,7 @@
         <v>1</v>
       </c>
       <c r="C220" s="1" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D220" s="1" t="s">
         <v>15</v>
@@ -6174,7 +6187,7 @@
         <v>1</v>
       </c>
       <c r="C221" s="1" t="n">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D221" s="1" t="s">
         <v>15</v>
@@ -6201,7 +6214,7 @@
         <v>1</v>
       </c>
       <c r="C222" s="1" t="n">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D222" s="1" t="s">
         <v>15</v>
@@ -6228,7 +6241,7 @@
         <v>1</v>
       </c>
       <c r="C223" s="1" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D223" s="1" t="s">
         <v>15</v>
@@ -6255,7 +6268,7 @@
         <v>1</v>
       </c>
       <c r="C224" s="1" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D224" s="1" t="s">
         <v>15</v>
@@ -6282,7 +6295,7 @@
         <v>1</v>
       </c>
       <c r="C225" s="1" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D225" s="1" t="s">
         <v>15</v>
@@ -6309,7 +6322,7 @@
         <v>1</v>
       </c>
       <c r="C226" s="1" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D226" s="1" t="s">
         <v>15</v>
@@ -6336,7 +6349,7 @@
         <v>1</v>
       </c>
       <c r="C227" s="1" t="n">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D227" s="1" t="s">
         <v>15</v>
@@ -6363,7 +6376,7 @@
         <v>1</v>
       </c>
       <c r="C228" s="1" t="n">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D228" s="1" t="s">
         <v>15</v>
@@ -6390,7 +6403,7 @@
         <v>1</v>
       </c>
       <c r="C229" s="1" t="n">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D229" s="1" t="s">
         <v>15</v>
@@ -6417,7 +6430,7 @@
         <v>1</v>
       </c>
       <c r="C230" s="1" t="n">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D230" s="1" t="s">
         <v>15</v>
@@ -6444,7 +6457,7 @@
         <v>1</v>
       </c>
       <c r="C231" s="1" t="n">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D231" s="1" t="s">
         <v>15</v>
@@ -6471,7 +6484,7 @@
         <v>1</v>
       </c>
       <c r="C232" s="1" t="n">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D232" s="1" t="s">
         <v>15</v>
@@ -6498,7 +6511,7 @@
         <v>1</v>
       </c>
       <c r="C233" s="1" t="n">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D233" s="1" t="s">
         <v>15</v>
@@ -6525,7 +6538,7 @@
         <v>1</v>
       </c>
       <c r="C234" s="1" t="n">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D234" s="1" t="s">
         <v>15</v>
@@ -6552,7 +6565,7 @@
         <v>1</v>
       </c>
       <c r="C235" s="1" t="n">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D235" s="1" t="s">
         <v>15</v>
@@ -6579,7 +6592,7 @@
         <v>1</v>
       </c>
       <c r="C236" s="1" t="n">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D236" s="1" t="s">
         <v>15</v>
@@ -6606,7 +6619,7 @@
         <v>1</v>
       </c>
       <c r="C237" s="1" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D237" s="1" t="s">
         <v>15</v>
@@ -6633,7 +6646,7 @@
         <v>1</v>
       </c>
       <c r="C238" s="1" t="n">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D238" s="1" t="s">
         <v>15</v>
@@ -6660,7 +6673,7 @@
         <v>1</v>
       </c>
       <c r="C239" s="1" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D239" s="1" t="s">
         <v>15</v>
@@ -6687,7 +6700,7 @@
         <v>1</v>
       </c>
       <c r="C240" s="1" t="n">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D240" s="1" t="s">
         <v>15</v>
@@ -6714,7 +6727,7 @@
         <v>1</v>
       </c>
       <c r="C241" s="1" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D241" s="1" t="s">
         <v>15</v>
@@ -6741,7 +6754,7 @@
         <v>1</v>
       </c>
       <c r="C242" s="1" t="n">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D242" s="1" t="s">
         <v>15</v>
@@ -6768,7 +6781,7 @@
         <v>1</v>
       </c>
       <c r="C243" s="1" t="n">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D243" s="1" t="s">
         <v>15</v>
@@ -6795,7 +6808,7 @@
         <v>1</v>
       </c>
       <c r="C244" s="1" t="n">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D244" s="1" t="s">
         <v>15</v>
@@ -6812,6 +6825,330 @@
       <c r="H244" s="1" t="n">
         <f aca="false">H242+1</f>
         <v>119</v>
+      </c>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A245" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B245" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C245" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="D245" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E245" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F245" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G245" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H245" s="1" t="n">
+        <f aca="false">H243+1</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A246" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B246" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C246" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="D246" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E246" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F246" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G246" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H246" s="1" t="n">
+        <f aca="false">H244+1</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A247" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B247" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C247" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="D247" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G247" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H247" s="1" t="n">
+        <f aca="false">H245+1</f>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A248" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B248" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C248" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="D248" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E248" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G248" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H248" s="1" t="n">
+        <f aca="false">H246+1</f>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A249" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B249" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C249" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="D249" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E249" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G249" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H249" s="1" t="n">
+        <f aca="false">H247+1</f>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A250" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B250" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C250" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="D250" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E250" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F250" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G250" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H250" s="1" t="n">
+        <f aca="false">H248+1</f>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A251" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B251" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C251" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="D251" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E251" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F251" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G251" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H251" s="1" t="n">
+        <f aca="false">H249+1</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A252" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B252" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C252" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E252" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F252" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G252" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H252" s="1" t="n">
+        <f aca="false">H250+1</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A253" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B253" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C253" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="D253" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E253" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F253" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G253" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H253" s="1" t="n">
+        <f aca="false">H251+1</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A254" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B254" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C254" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="D254" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E254" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F254" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G254" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H254" s="1" t="n">
+        <f aca="false">H252+1</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A255" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B255" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C255" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="D255" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E255" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F255" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G255" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H255" s="1" t="n">
+        <f aca="false">H253+1</f>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A256" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B256" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C256" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="D256" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E256" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F256" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G256" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H256" s="1" t="n">
+        <f aca="false">H254+1</f>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EMTF_vu13p in progress, getting exception in mgt_builder.jar
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/link_map_vu13p_gty.xlsx
+++ b/examples/vu13p_25g_all/src/link_map_vu13p_gty.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AXI_X0Y24_Y30" sheetId="1" state="visible" r:id="rId2"/>
@@ -249,7 +249,7 @@
   </sheetPr>
   <dimension ref="A1:I256"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -7174,7 +7174,7 @@
   </sheetPr>
   <dimension ref="A1:I256"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -14124,7 +14124,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
proper TCDS connection mapping in 25G all link test
</commit_message>
<xml_diff>
--- a/examples/vu13p_25g_all/src/link_map_vu13p_gty.xlsx
+++ b/examples/vu13p_25g_all/src/link_map_vu13p_gty.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="AXI_X0Y24_Y30" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="AXI_X0Y0_Y4" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="AXI_X0Y18_Y20" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Proper_TCDS" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3915" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3911" uniqueCount="34">
   <si>
     <t xml:space="preserve">boards/vu13p_gty</t>
   </si>
@@ -125,9 +125,6 @@
   <si>
     <t xml:space="preserve">//tx</t>
   </si>
-  <si>
-    <t xml:space="preserve">axi</t>
-  </si>
 </sst>
 </file>
 
@@ -221,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -247,10 +244,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -14221,8 +14214,8 @@
   </sheetPr>
   <dimension ref="A1:I260"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H47" activeCellId="0" sqref="H47"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I52" activeCellId="0" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14522,26 +14515,26 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" s="7" t="n">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1" t="n">
         <f aca="false">C15-1</f>
         <v>4</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="H13" s="1" t="n">
@@ -14550,26 +14543,26 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="7" t="n">
+      <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1" t="n">
         <f aca="false">C16-1</f>
         <v>4</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="D14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>19</v>
       </c>
       <c r="H14" s="1" t="n">
@@ -15195,7 +15188,7 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B37" s="6" t="n">
         <v>0</v>
@@ -15216,10 +15209,13 @@
       <c r="G37" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="H37" s="1" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B38" s="6" t="n">
         <v>0</v>
@@ -15240,10 +15236,13 @@
       <c r="G38" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="H38" s="1" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B39" s="6" t="n">
         <v>0</v>
@@ -15264,10 +15263,14 @@
       <c r="G39" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="H39" s="1" t="n">
+        <f aca="false">H37+1</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B40" s="6" t="n">
         <v>0</v>
@@ -15288,10 +15291,14 @@
       <c r="G40" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="H40" s="1" t="n">
+        <f aca="false">H38+1</f>
+        <v>17</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B41" s="6" t="n">
         <v>0</v>
@@ -15312,13 +15319,14 @@
       <c r="G41" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>34</v>
+      <c r="H41" s="1" t="n">
+        <f aca="false">H39+1</f>
+        <v>18</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B42" s="6" t="n">
         <v>0</v>
@@ -15339,13 +15347,14 @@
       <c r="G42" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H42" s="1" t="s">
-        <v>34</v>
+      <c r="H42" s="1" t="n">
+        <f aca="false">H40+1</f>
+        <v>18</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B43" s="6" t="n">
         <v>0</v>
@@ -15366,10 +15375,14 @@
       <c r="G43" s="6" t="s">
         <v>17</v>
       </c>
+      <c r="H43" s="1" t="n">
+        <f aca="false">H41+1</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="B44" s="6" t="n">
         <v>0</v>
@@ -15390,10 +15403,14 @@
       <c r="G44" s="6" t="s">
         <v>19</v>
       </c>
+      <c r="H44" s="1" t="n">
+        <f aca="false">H42+1</f>
+        <v>19</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="s">
-        <v>32</v>
+      <c r="A45" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>0</v>
@@ -15414,13 +15431,14 @@
       <c r="G45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H45" s="1" t="s">
-        <v>34</v>
+      <c r="H45" s="1" t="n">
+        <f aca="false">H43+1</f>
+        <v>20</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="s">
-        <v>33</v>
+      <c r="A46" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>0</v>
@@ -15441,13 +15459,14 @@
       <c r="G46" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>34</v>
+      <c r="H46" s="1" t="n">
+        <f aca="false">H44+1</f>
+        <v>20</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="s">
-        <v>32</v>
+      <c r="A47" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>0</v>
@@ -15468,10 +15487,14 @@
       <c r="G47" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H47" s="1" t="n">
+        <f aca="false">H45+1</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="s">
-        <v>33</v>
+      <c r="A48" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>0</v>
@@ -15492,10 +15515,14 @@
       <c r="G48" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H48" s="1" t="n">
+        <f aca="false">H46+1</f>
+        <v>21</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="s">
-        <v>32</v>
+      <c r="A49" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>0</v>
@@ -15516,10 +15543,14 @@
       <c r="G49" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H49" s="1" t="n">
+        <f aca="false">H47+1</f>
+        <v>22</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="s">
-        <v>33</v>
+      <c r="A50" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>0</v>
@@ -15540,10 +15571,14 @@
       <c r="G50" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H50" s="1" t="n">
+        <f aca="false">H48+1</f>
+        <v>22</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="s">
-        <v>32</v>
+      <c r="A51" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>0</v>
@@ -15564,10 +15599,14 @@
       <c r="G51" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H51" s="1" t="n">
+        <f aca="false">H49+1</f>
+        <v>23</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
-        <v>33</v>
+      <c r="A52" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B52" s="1" t="n">
         <v>0</v>
@@ -15588,10 +15627,14 @@
       <c r="G52" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="H52" s="1" t="n">
+        <f aca="false">H50+1</f>
+        <v>23</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="6" t="s">
-        <v>12</v>
+      <c r="A53" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B53" s="6" t="n">
         <v>0</v>
@@ -15612,13 +15655,11 @@
       <c r="G53" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H53" s="1" t="n">
-        <v>16</v>
-      </c>
+      <c r="H53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="6" t="s">
-        <v>18</v>
+      <c r="A54" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B54" s="6" t="n">
         <v>0</v>
@@ -15639,13 +15680,11 @@
       <c r="G54" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H54" s="1" t="n">
-        <v>16</v>
-      </c>
+      <c r="H54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="6" t="s">
-        <v>12</v>
+      <c r="A55" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B55" s="6" t="n">
         <v>0</v>
@@ -15666,14 +15705,11 @@
       <c r="G55" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H55" s="1" t="n">
-        <f aca="false">H53+1</f>
-        <v>17</v>
-      </c>
+      <c r="H55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6" t="s">
-        <v>18</v>
+      <c r="A56" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B56" s="6" t="n">
         <v>0</v>
@@ -15694,14 +15730,11 @@
       <c r="G56" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H56" s="1" t="n">
-        <f aca="false">H54+1</f>
-        <v>17</v>
-      </c>
+      <c r="H56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
-        <v>12</v>
+      <c r="A57" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B57" s="6" t="n">
         <v>0</v>
@@ -15722,14 +15755,11 @@
       <c r="G57" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H57" s="1" t="n">
-        <f aca="false">H55+1</f>
-        <v>18</v>
-      </c>
+      <c r="H57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6" t="s">
-        <v>18</v>
+      <c r="A58" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B58" s="6" t="n">
         <v>0</v>
@@ -15750,14 +15780,11 @@
       <c r="G58" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H58" s="1" t="n">
-        <f aca="false">H56+1</f>
-        <v>18</v>
-      </c>
+      <c r="H58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="6" t="s">
-        <v>12</v>
+      <c r="A59" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B59" s="6" t="n">
         <v>0</v>
@@ -15778,14 +15805,11 @@
       <c r="G59" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H59" s="1" t="n">
-        <f aca="false">H57+1</f>
-        <v>19</v>
-      </c>
+      <c r="H59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="6" t="s">
-        <v>18</v>
+      <c r="A60" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B60" s="6" t="n">
         <v>0</v>
@@ -15806,14 +15830,11 @@
       <c r="G60" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H60" s="1" t="n">
-        <f aca="false">H58+1</f>
-        <v>19</v>
-      </c>
+      <c r="H60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B61" s="1" t="n">
         <v>0</v>
@@ -15834,14 +15855,11 @@
       <c r="G61" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H61" s="1" t="n">
-        <f aca="false">H59+1</f>
-        <v>20</v>
-      </c>
+      <c r="H61" s="0"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B62" s="1" t="n">
         <v>0</v>
@@ -15862,14 +15880,11 @@
       <c r="G62" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H62" s="1" t="n">
-        <f aca="false">H60+1</f>
-        <v>20</v>
-      </c>
+      <c r="H62" s="0"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B63" s="1" t="n">
         <v>0</v>
@@ -15890,14 +15905,11 @@
       <c r="G63" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H63" s="1" t="n">
-        <f aca="false">H61+1</f>
-        <v>21</v>
-      </c>
+      <c r="H63" s="0"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B64" s="1" t="n">
         <v>0</v>
@@ -15918,14 +15930,11 @@
       <c r="G64" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H64" s="1" t="n">
-        <f aca="false">H62+1</f>
-        <v>21</v>
-      </c>
+      <c r="H64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B65" s="1" t="n">
         <v>0</v>
@@ -15946,14 +15955,11 @@
       <c r="G65" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H65" s="1" t="n">
-        <f aca="false">H63+1</f>
-        <v>22</v>
-      </c>
+      <c r="H65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B66" s="1" t="n">
         <v>0</v>
@@ -15974,14 +15980,11 @@
       <c r="G66" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H66" s="1" t="n">
-        <f aca="false">H64+1</f>
-        <v>22</v>
-      </c>
+      <c r="H66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B67" s="1" t="n">
         <v>0</v>
@@ -16001,14 +16004,11 @@
       <c r="G67" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H67" s="1" t="n">
-        <f aca="false">H65+1</f>
-        <v>23</v>
-      </c>
+      <c r="H67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B68" s="1" t="n">
         <v>0</v>
@@ -16028,10 +16028,7 @@
       <c r="G68" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H68" s="1" t="n">
-        <f aca="false">H66+1</f>
-        <v>23</v>
-      </c>
+      <c r="H68" s="0"/>
       <c r="I68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16057,7 +16054,7 @@
         <v>17</v>
       </c>
       <c r="H69" s="1" t="n">
-        <f aca="false">H67+1</f>
+        <f aca="false">H51+1</f>
         <v>24</v>
       </c>
     </row>
@@ -16084,7 +16081,7 @@
         <v>19</v>
       </c>
       <c r="H70" s="1" t="n">
-        <f aca="false">H68+1</f>
+        <f aca="false">H52+1</f>
         <v>24</v>
       </c>
     </row>

</xml_diff>